<commit_message>
ESG-Fx test sequence generation for Edge Coverage is added, Automatic Product Congiguration with SAT Solvers is added, Feature Model parser is updated.
yes
</commit_message>
<xml_diff>
--- a/files/Cases/SodaVendingMachine/SVM.xlsx
+++ b/files/Cases/SodaVendingMachine/SVM.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dilekozturk/git/esg-with-feature-expressions/files/Cases/SodaVendingMachine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5073EF2-69B8-0640-8FF5-59B50C24C04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B502E91-862F-804E-8691-7D037B487FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" activeTab="1" xr2:uid="{59776E75-10D5-E346-BDF3-27068CE50C7E}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17300" activeTab="1" xr2:uid="{59776E75-10D5-E346-BDF3-27068CE50C7E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sayfa2" sheetId="2" r:id="rId2"/>
+    <sheet name="EventCoverage_TestGeneration" sheetId="1" r:id="rId1"/>
+    <sheet name="EventCoverage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="65">
   <si>
     <t>SVM</t>
   </si>
@@ -236,13 +236,19 @@
     <t>7 : pay, change, soda, serveSoda, open, take, close
 4 : free, tea, serveTea, take
 3 : free, cancel, return</t>
+  </si>
+  <si>
+    <t>Number of Test Sequences</t>
+  </si>
+  <si>
+    <t>Number of Events</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,6 +296,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -323,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -360,17 +372,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -521,83 +522,73 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -670,6 +661,48 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -690,9 +723,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -730,7 +763,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -836,7 +869,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -978,7 +1011,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -986,235 +1019,238 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A45C49-5DF4-C843-918F-D53AF3971298}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M155"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="57.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="58.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>18.46</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>17.23</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>14.12</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>15.07</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>18.53</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>15.31</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>13.31</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>15.79</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>13.83</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>13.62</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <f>AVERAGE(B2:B11)</f>
         <v>15.527000000000001</v>
       </c>
@@ -1231,8 +1267,8 @@
       <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="20"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1246,1108 +1282,1108 @@
       <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>16.440000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <v>13.77</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>13.59</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>13.57</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>15.08</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>16.97</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>14.25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>13.82</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="9">
         <v>15.47</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <v>15.35</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <f>AVERAGE(B15:B24)</f>
         <v>14.831</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="20"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="19"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="9">
         <v>18.02</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="9">
         <v>16.809999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <v>17.04</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="9">
         <v>16.07</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="9">
         <v>16.190000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="9">
         <v>16.190000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="9">
         <v>16.989999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="13">
+      <c r="B35" s="12">
         <v>17.02</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="9">
         <v>16.45</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="9">
         <v>15.91</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="11">
+      <c r="B38" s="10">
         <f>AVERAGE(B28:B37)</f>
         <v>16.668999999999997</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="19"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="9">
         <v>16.38</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="9">
         <v>14.58</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="13">
+      <c r="B43" s="12">
         <v>14.04</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="9">
         <v>14.35</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="9">
         <v>15.63</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="10">
+      <c r="B46" s="9">
         <v>14.33</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="13">
+      <c r="B47" s="12">
         <v>14.05</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="10">
+      <c r="B48" s="9">
         <v>13.92</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="9">
         <v>14.01</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B50" s="10">
+      <c r="B50" s="9">
         <v>15.36</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51" s="10">
         <f>AVERAGE(B41:B50)</f>
         <v>14.664999999999997</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="20"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="19"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="10">
+      <c r="B54" s="9">
         <v>16.989999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B55" s="10">
+      <c r="B55" s="9">
         <v>15.35</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B56" s="10">
+      <c r="B56" s="9">
         <v>14.94</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B57" s="13">
+      <c r="B57" s="12">
         <v>14.07</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B58" s="10">
+      <c r="B58" s="9">
         <v>14.86</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="13">
+      <c r="B59" s="12">
         <v>14.09</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B60" s="10">
+      <c r="B60" s="9">
         <v>13.87</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B61" s="10">
+      <c r="B61" s="9">
         <v>20.64</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B62" s="13">
+      <c r="B62" s="12">
         <v>14.11</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B63" s="14">
+      <c r="B63" s="13">
         <v>14.73</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="17">
+      <c r="B64" s="16">
         <f>AVERAGE(B54:B63)</f>
         <v>15.365</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="22"/>
-      <c r="B65" s="20"/>
+      <c r="A65" s="21"/>
+      <c r="B65" s="19"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B67" s="10">
+      <c r="B67" s="9">
         <v>15.87</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B68" s="13">
+      <c r="B68" s="12">
         <v>17.05</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="7" t="s">
+      <c r="A69" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B69" s="10">
+      <c r="B69" s="9">
         <v>14.96</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B70" s="10">
+      <c r="B70" s="9">
         <v>16.34</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B71" s="10">
+      <c r="B71" s="9">
         <v>14.51</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B72" s="10">
+      <c r="B72" s="9">
         <v>16.920000000000002</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B73" s="10">
+      <c r="B73" s="9">
         <v>14.99</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B74" s="10">
+      <c r="B74" s="9">
         <v>14.54</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B75" s="10">
+      <c r="B75" s="9">
         <v>14.45</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B76" s="10">
+      <c r="B76" s="9">
         <v>14.66</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="18" t="s">
+      <c r="A77" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B77" s="11">
+      <c r="B77" s="10">
         <f>AVERAGE(B67:B76)</f>
         <v>15.428999999999998</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="19"/>
-      <c r="B78" s="23"/>
+      <c r="A78" s="18"/>
+      <c r="B78" s="22"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
+      <c r="A79" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B79" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B80" s="10">
+      <c r="B80" s="9">
         <v>17.53</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B81" s="10">
+      <c r="B81" s="9">
         <v>14.34</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B82" s="10">
+      <c r="B82" s="9">
         <v>15.31</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B83" s="10">
+      <c r="B83" s="9">
         <v>15.72</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B84" s="10">
+      <c r="B84" s="9">
         <v>15.83</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B85" s="13">
+      <c r="B85" s="12">
         <v>14.09</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="7" t="s">
+      <c r="A86" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B86" s="10">
+      <c r="B86" s="9">
         <v>14.97</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="7" t="s">
+      <c r="A87" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B87" s="10">
+      <c r="B87" s="9">
         <v>15.27</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B88" s="10">
+      <c r="B88" s="9">
         <v>14.78</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B89" s="10">
+      <c r="B89" s="9">
         <v>15.73</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="18" t="s">
+      <c r="A90" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B90" s="11">
+      <c r="B90" s="10">
         <f>AVERAGE(B80:B89)</f>
         <v>15.356999999999999</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="19"/>
-      <c r="B91" s="23"/>
+      <c r="A91" s="18"/>
+      <c r="B91" s="22"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="6" t="s">
+      <c r="A92" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B92" s="9" t="s">
+      <c r="B92" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="7" t="s">
+      <c r="A93" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B93" s="10">
+      <c r="B93" s="9">
         <v>18.850000000000001</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B94" s="10">
+      <c r="B94" s="9">
         <v>17.170000000000002</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="7" t="s">
+      <c r="A95" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B95" s="10">
+      <c r="B95" s="9">
         <v>17.59</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="7" t="s">
+      <c r="A96" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B96" s="10">
+      <c r="B96" s="9">
         <v>17.41</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="7" t="s">
+      <c r="A97" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B97" s="10">
+      <c r="B97" s="9">
         <v>19.22</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="7" t="s">
+      <c r="A98" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="10">
+      <c r="B98" s="9">
         <v>17.47</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="7" t="s">
+      <c r="A99" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B99" s="10">
+      <c r="B99" s="9">
         <v>18.420000000000002</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="7" t="s">
+      <c r="A100" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B100" s="10">
+      <c r="B100" s="9">
         <v>18.79</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="7" t="s">
+      <c r="A101" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B101" s="10">
+      <c r="B101" s="9">
         <v>16.98</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="7" t="s">
+      <c r="A102" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B102" s="10">
+      <c r="B102" s="9">
         <v>17.850000000000001</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="18" t="s">
+      <c r="A103" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B103" s="11">
+      <c r="B103" s="10">
         <f>AVERAGE(B93:B102)</f>
         <v>17.974999999999998</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="19"/>
-      <c r="B104" s="23"/>
+      <c r="A104" s="18"/>
+      <c r="B104" s="22"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="6" t="s">
+      <c r="A105" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B105" s="9" t="s">
+      <c r="B105" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="7" t="s">
+      <c r="A106" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B106" s="10">
+      <c r="B106" s="9">
         <v>16.87</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="7" t="s">
+      <c r="A107" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B107" s="13">
+      <c r="B107" s="12">
         <v>15.05</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="7" t="s">
+      <c r="A108" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B108" s="10">
+      <c r="B108" s="9">
         <v>13.65</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="7" t="s">
+      <c r="A109" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B109" s="10">
+      <c r="B109" s="9">
         <v>14.58</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="7" t="s">
+      <c r="A110" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B110" s="10">
+      <c r="B110" s="9">
         <v>14.63</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="7" t="s">
+      <c r="A111" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B111" s="13">
+      <c r="B111" s="12">
         <v>14.09</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="7" t="s">
+      <c r="A112" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B112" s="10">
+      <c r="B112" s="9">
         <v>19.64</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="7" t="s">
+      <c r="A113" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B113" s="10">
+      <c r="B113" s="9">
         <v>14.21</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
+      <c r="A114" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B114" s="10">
+      <c r="B114" s="9">
         <v>14.42</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="7" t="s">
+      <c r="A115" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B115" s="10">
+      <c r="B115" s="9">
         <v>14.63</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="18" t="s">
+      <c r="A116" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B116" s="11">
+      <c r="B116" s="10">
         <f>AVERAGE(B106:B115)</f>
         <v>15.176999999999998</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="19"/>
-      <c r="B117" s="23"/>
+      <c r="A117" s="18"/>
+      <c r="B117" s="22"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="6" t="s">
+      <c r="A118" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B118" s="9" t="s">
+      <c r="B118" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="7" t="s">
+      <c r="A119" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B119" s="10">
+      <c r="B119" s="9">
         <v>17.37</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="7" t="s">
+      <c r="A120" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B120" s="10">
+      <c r="B120" s="9">
         <v>20.96</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="7" t="s">
+      <c r="A121" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B121" s="10">
+      <c r="B121" s="9">
         <v>15.31</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="7" t="s">
+      <c r="A122" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B122" s="13">
+      <c r="B122" s="12">
         <v>15.01</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="7" t="s">
+      <c r="A123" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B123" s="10">
+      <c r="B123" s="9">
         <v>15</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="7" t="s">
+      <c r="A124" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B124" s="10">
+      <c r="B124" s="9">
         <v>14.79</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="7" t="s">
+      <c r="A125" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B125" s="10">
+      <c r="B125" s="9">
         <v>14.38</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="7" t="s">
+      <c r="A126" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B126" s="13">
+      <c r="B126" s="12">
         <v>16.059999999999999</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="7" t="s">
+      <c r="A127" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B127" s="13">
+      <c r="B127" s="12">
         <v>14.12</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="7" t="s">
+      <c r="A128" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B128" s="10">
+      <c r="B128" s="9">
         <v>14.38</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="18" t="s">
+      <c r="A129" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B129" s="11">
+      <c r="B129" s="10">
         <f>AVERAGE(B119:B128)</f>
         <v>15.738</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="19"/>
-      <c r="B130" s="23"/>
+      <c r="A130" s="18"/>
+      <c r="B130" s="22"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="6" t="s">
+      <c r="A131" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B131" s="9" t="s">
+      <c r="B131" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="7" t="s">
+      <c r="A132" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B132" s="10">
+      <c r="B132" s="9">
         <v>17.739999999999998</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="7" t="s">
+      <c r="A133" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B133" s="10">
+      <c r="B133" s="9">
         <v>16</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" s="7" t="s">
+      <c r="A134" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B134" s="10">
+      <c r="B134" s="9">
         <v>15.42</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="7" t="s">
+      <c r="A135" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B135" s="10">
+      <c r="B135" s="9">
         <v>15.42</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="7" t="s">
+      <c r="A136" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B136" s="10">
+      <c r="B136" s="9">
         <v>14.74</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="7" t="s">
+      <c r="A137" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B137" s="10">
+      <c r="B137" s="9">
         <v>14.77</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="7" t="s">
+      <c r="A138" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B138" s="13">
+      <c r="B138" s="12">
         <v>15.06</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="7" t="s">
+      <c r="A139" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B139" s="10">
+      <c r="B139" s="9">
         <v>16.190000000000001</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="7" t="s">
+      <c r="A140" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B140" s="13">
+      <c r="B140" s="12">
         <v>14.05</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="7" t="s">
+      <c r="A141" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B141" s="10">
+      <c r="B141" s="9">
         <v>14.52</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="18" t="s">
+      <c r="A142" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B142" s="11">
+      <c r="B142" s="10">
         <f>AVERAGE(B132:B141)</f>
         <v>15.391</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="19"/>
-      <c r="B143" s="23"/>
+      <c r="A143" s="18"/>
+      <c r="B143" s="22"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="6" t="s">
+      <c r="A144" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B144" s="9" t="s">
+      <c r="B144" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="7" t="s">
+      <c r="A145" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B145" s="10">
+      <c r="B145" s="9">
         <v>15.26</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="7" t="s">
+      <c r="A146" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B146" s="10">
+      <c r="B146" s="9">
         <v>14.42</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="7" t="s">
+      <c r="A147" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B147" s="10">
+      <c r="B147" s="9">
         <v>15.47</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="7" t="s">
+      <c r="A148" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B148" s="10">
+      <c r="B148" s="9">
         <v>15.19</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="7" t="s">
+      <c r="A149" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B149" s="10">
+      <c r="B149" s="9">
         <v>14.55</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="7" t="s">
+      <c r="A150" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B150" s="10">
+      <c r="B150" s="9">
         <v>14.84</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="7" t="s">
+      <c r="A151" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B151" s="10">
+      <c r="B151" s="9">
         <v>15.78</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="7" t="s">
+      <c r="A152" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B152" s="10">
+      <c r="B152" s="9">
         <v>14.38</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="7" t="s">
+      <c r="A153" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B153" s="10">
+      <c r="B153" s="9">
         <v>14.61</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="7" t="s">
+      <c r="A154" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B154" s="13">
+      <c r="B154" s="12">
         <v>14.07</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="18" t="s">
+      <c r="A155" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B155" s="11">
+      <c r="B155" s="10">
         <f>AVERAGE(B145:B154)</f>
         <v>14.856999999999999</v>
       </c>
@@ -2355,320 +2391,411 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="31" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E6B7AC-743F-714B-B1B2-A4AC8BB60302}">
-  <dimension ref="A1:Q24"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="56" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5" style="54" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="57" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" style="56" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="H1" s="23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="26">
         <v>1</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E2" s="26">
         <v>1</v>
       </c>
-      <c r="F2" s="32">
-        <f>Sayfa1!B12</f>
+      <c r="F2" s="26">
+        <v>7</v>
+      </c>
+      <c r="G2" s="27">
+        <v>1</v>
+      </c>
+      <c r="H2" s="28">
+        <f>EventCoverage_TestGeneration!B12</f>
         <v>15.527000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="26">
         <v>1</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="26">
         <v>1</v>
       </c>
-      <c r="F3" s="32">
-        <f>Sayfa1!B25</f>
+      <c r="F3" s="26">
+        <v>7</v>
+      </c>
+      <c r="G3" s="27">
+        <v>1</v>
+      </c>
+      <c r="H3" s="28">
+        <f>EventCoverage_TestGeneration!B25</f>
         <v>14.831</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="31">
         <v>2</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="49">
+        <v>2</v>
+      </c>
+      <c r="F4" s="49">
+        <v>14</v>
+      </c>
+      <c r="G4" s="33">
         <v>1</v>
       </c>
-      <c r="F4" s="38">
-        <f>Sayfa1!B38</f>
+      <c r="H4" s="34">
+        <f>EventCoverage_TestGeneration!B38</f>
         <v>16.668999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="31">
         <v>2</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="31">
         <v>1</v>
       </c>
-      <c r="F5" s="38">
-        <f>Sayfa1!B51</f>
+      <c r="F5" s="31">
+        <v>4</v>
+      </c>
+      <c r="G5" s="33">
+        <v>1</v>
+      </c>
+      <c r="H5" s="34">
+        <f>EventCoverage_TestGeneration!B51</f>
         <v>14.664999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="31">
         <v>2</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E6" s="31">
         <v>1</v>
       </c>
-      <c r="F6" s="38">
-        <f>Sayfa1!B64</f>
+      <c r="F6" s="31">
+        <v>4</v>
+      </c>
+      <c r="G6" s="33">
+        <v>1</v>
+      </c>
+      <c r="H6" s="34">
+        <f>EventCoverage_TestGeneration!B64</f>
         <v>15.365</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="39" t="s">
+    <row r="7" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="31">
         <v>2</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="49">
+        <v>2</v>
+      </c>
+      <c r="F7" s="49">
+        <v>11</v>
+      </c>
+      <c r="G7" s="33">
         <v>1</v>
       </c>
-      <c r="F7" s="38">
-        <f>Sayfa1!B77</f>
+      <c r="H7" s="34">
+        <f>EventCoverage_TestGeneration!B77</f>
         <v>15.428999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="31">
         <v>2</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="49">
+        <v>2</v>
+      </c>
+      <c r="F8" s="49">
+        <v>11</v>
+      </c>
+      <c r="G8" s="33">
         <v>1</v>
       </c>
-      <c r="F8" s="38">
-        <f>Sayfa1!B90</f>
+      <c r="H8" s="34">
+        <f>EventCoverage_TestGeneration!B90</f>
         <v>15.356999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="40" t="s">
+    <row r="9" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="38">
         <v>3</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="50">
+        <v>3</v>
+      </c>
+      <c r="F9" s="50">
+        <v>18</v>
+      </c>
+      <c r="G9" s="40">
         <v>1</v>
       </c>
-      <c r="F9" s="45">
-        <f>Sayfa1!B103</f>
+      <c r="H9" s="41">
+        <f>EventCoverage_TestGeneration!B103</f>
         <v>17.974999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
+    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="38">
         <v>3</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="50">
+        <v>2</v>
+      </c>
+      <c r="F10" s="50">
+        <v>7</v>
+      </c>
+      <c r="G10" s="40">
         <v>1</v>
       </c>
-      <c r="F10" s="45">
-        <f>Sayfa1!B116</f>
+      <c r="H10" s="41">
+        <f>EventCoverage_TestGeneration!B116</f>
         <v>15.176999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
+    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="42">
+      <c r="C11" s="38">
         <v>3</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="50">
+        <v>2</v>
+      </c>
+      <c r="F11" s="50">
+        <v>7</v>
+      </c>
+      <c r="G11" s="40">
         <v>1</v>
       </c>
-      <c r="F11" s="45">
-        <f>Sayfa1!B129</f>
+      <c r="H11" s="41">
+        <f>EventCoverage_TestGeneration!B129</f>
         <v>15.738</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
+    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="42">
+      <c r="C12" s="38">
         <v>3</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="50">
+        <v>2</v>
+      </c>
+      <c r="F12" s="50">
+        <v>8</v>
+      </c>
+      <c r="G12" s="40">
         <v>1</v>
       </c>
-      <c r="F12" s="45">
-        <f>Sayfa1!B142</f>
+      <c r="H12" s="41">
+        <f>EventCoverage_TestGeneration!B142</f>
         <v>15.391</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
+    <row r="13" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="48">
+      <c r="C13" s="44">
         <v>4</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="50">
+      <c r="E13" s="51">
+        <v>3</v>
+      </c>
+      <c r="F13" s="51">
+        <v>14</v>
+      </c>
+      <c r="G13" s="46">
         <v>1</v>
       </c>
-      <c r="F13" s="51">
-        <f>Sayfa1!B155</f>
+      <c r="H13" s="47">
+        <f>EventCoverage_TestGeneration!B155</f>
         <v>14.856999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-    </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-    </row>
-    <row r="24" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D24" s="3"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G14" s="58"/>
+      <c r="H14" s="59">
+        <f>AVERAGE(H2:H13)</f>
+        <v>15.58175</v>
+      </c>
+    </row>
+    <row r="21" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="60"/>
+      <c r="R21" s="60"/>
+      <c r="S21" s="60"/>
+    </row>
+    <row r="24" spans="4:19" x14ac:dyDescent="0.2">
+      <c r="D24" s="55"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="67" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>